<commit_message>
fixed writing into excel method
</commit_message>
<xml_diff>
--- a/Data/EmployeeSalaryData.xlsx
+++ b/Data/EmployeeSalaryData.xlsx
@@ -2,17 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
   <sheets>
     <sheet state="visible" name="dataSalary" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="dataInfo" sheetId="2" r:id="rId5"/>
   </sheets>
-  <definedNames/>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="31">
   <si>
     <t>EMPID</t>
   </si>
@@ -99,12 +101,19 @@
   </si>
   <si>
     <t>EMAIL</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Passed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="10.0"/>
@@ -353,6 +362,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -564,12 +574,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="4" max="4" width="26.43"/>
+    <col min="4" max="4" customWidth="true" width="26.43" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -735,6 +746,9 @@
         <f t="shared" si="1"/>
         <v>NEIOENLLEN@gmail.com</v>
       </c>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1">

</xml_diff>

<commit_message>
updates for util classes, autoit, reading fron excel, actionclass, robot class
</commit_message>
<xml_diff>
--- a/Data/EmployeeSalaryData.xlsx
+++ b/Data/EmployeeSalaryData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="34">
   <si>
     <t>EMPID</t>
   </si>
@@ -103,10 +103,19 @@
     <t>EMAIL</t>
   </si>
   <si>
+    <t>RESULT1</t>
+  </si>
+  <si>
+    <t>RESULT2</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
     <t>Failed</t>
-  </si>
-  <si>
-    <t>Passed</t>
   </si>
 </sst>
 </file>
@@ -574,7 +583,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -596,6 +605,12 @@
       <c r="D1" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
@@ -747,7 +762,10 @@
         <v>NEIOENLLEN@gmail.com</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>32</v>
+      </c>
+      <c r="G11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12">

</xml_diff>